<commit_message>
Add hyperlinks to coverpage
</commit_message>
<xml_diff>
--- a/share_dinkum_proj/share_dinkum_app/import_data/data_import_template_public.xlsx
+++ b/share_dinkum_proj/share_dinkum_app/import_data/data_import_template_public.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED45DC35-D66F-48B5-AE04-438B5B51FAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02433E7E-7158-4E89-84A9-436E8AD16551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9819" uniqueCount="4827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9820" uniqueCount="4828">
   <si>
     <t>sheet_name</t>
   </si>
@@ -14523,6 +14523,9 @@
   </si>
   <si>
     <t>file</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
@@ -14532,7 +14535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14554,6 +14557,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -14588,14 +14598,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -14614,9 +14625,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="uuid" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
@@ -14688,19 +14701,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="table_info" displayName="table_info" ref="A1:D17">
-  <autoFilter ref="A1:D17" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="table_info" displayName="table_info" ref="A1:E17">
+  <autoFilter ref="A1:E17" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="sheet_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="table_name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="description"/>
     <tableColumn id="4" xr3:uid="{08F81B28-F2EE-45C1-B03F-C3CF7BC3C7F8}" name="available_for_import"/>
+    <tableColumn id="5" xr3:uid="{D0F52A90-199B-4C6F-A1C6-F797E2C155BA}" name="link" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15151,11 +15165,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15166,7 +15180,7 @@
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15179,8 +15193,11 @@
       <c r="D1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -15190,8 +15207,12 @@
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="str">
+        <f>HYPERLINK("#'01'!A1", "01")</f>
+        <v>01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -15201,8 +15222,12 @@
       <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="str">
+        <f>HYPERLINK("#'02'!A1", "02")</f>
+        <v>02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -15212,8 +15237,12 @@
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="str">
+        <f>HYPERLINK("#'03'!A1", "03")</f>
+        <v>03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -15223,8 +15252,12 @@
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="8" t="str">
+        <f>HYPERLINK("#'04'!A1", "04")</f>
+        <v>04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -15234,8 +15267,12 @@
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="8" t="str">
+        <f>HYPERLINK("#'05'!A1", "05")</f>
+        <v>05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -15248,8 +15285,12 @@
       <c r="D7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="8" t="str">
+        <f>HYPERLINK("#'06'!A1", "06")</f>
+        <v>06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -15262,8 +15303,12 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="8" t="str">
+        <f>HYPERLINK("#'07'!A1", "07")</f>
+        <v>07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -15276,8 +15321,12 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="8" t="str">
+        <f>HYPERLINK("#'08'!A1", "08")</f>
+        <v>08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -15290,8 +15339,12 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="8" t="str">
+        <f>HYPERLINK("#'09'!A1", "09")</f>
+        <v>09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -15301,8 +15354,12 @@
       <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="8" t="str">
+        <f>HYPERLINK("#'10'!A1", "10")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -15315,8 +15372,12 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="8" t="str">
+        <f>HYPERLINK("#'11'!A1", "11")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -15329,8 +15390,12 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="8" t="str">
+        <f>HYPERLINK("#'12'!A1", "12")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -15343,8 +15408,12 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="str">
+        <f>HYPERLINK("#'13'!A1", "13")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -15354,8 +15423,12 @@
       <c r="C15" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="str">
+        <f>HYPERLINK("#'14'!A1", "14")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -15368,8 +15441,12 @@
       <c r="D16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="8" t="str">
+        <f>HYPERLINK("#'15'!A1", "15")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -15381,6 +15458,10 @@
       </c>
       <c r="D17" t="b">
         <v>1</v>
+      </c>
+      <c r="E17" s="8" t="str">
+        <f>HYPERLINK("#'16'!A1", "16")</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>